<commit_message>
maodificacion de lectura de adc
se modifico la forma como va a leer el adc del esclavo
</commit_message>
<xml_diff>
--- a/Conexion de los pines de maestro.xlsx
+++ b/Conexion de los pines de maestro.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Arduino\proyecto Miller\proyectoMiller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E710DF-9889-4628-9FFA-EF44192856B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ED91340-81F3-416E-B6FD-9E7F9360D92B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A3430B96-D652-4A0A-8FC6-A3949DC225C1}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{A3430B96-D652-4A0A-8FC6-A3949DC225C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>uso</t>
   </si>
@@ -81,58 +81,139 @@
     <t>hd</t>
   </si>
   <si>
-    <t>D0.0</t>
-  </si>
-  <si>
-    <t>D0.3</t>
-  </si>
-  <si>
-    <t>D2</t>
-  </si>
-  <si>
-    <t>D0.1</t>
-  </si>
-  <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>D0.2</t>
-  </si>
-  <si>
-    <t>D3</t>
-  </si>
-  <si>
-    <t>D0</t>
-  </si>
-  <si>
-    <t>Luz 2</t>
-  </si>
-  <si>
-    <t>luz 4</t>
-  </si>
-  <si>
-    <t>Luz 3</t>
-  </si>
-  <si>
-    <t>Luz 5</t>
-  </si>
-  <si>
-    <t>Luz 7</t>
-  </si>
-  <si>
-    <t>Luz 8</t>
-  </si>
-  <si>
-    <t>Luz 16</t>
-  </si>
-  <si>
-    <t>Luz 6</t>
-  </si>
-  <si>
-    <t>Luz 11</t>
-  </si>
-  <si>
-    <t>Luz 12</t>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>a14</t>
+  </si>
+  <si>
+    <t>a13</t>
+  </si>
+  <si>
+    <t>a12</t>
+  </si>
+  <si>
+    <t>a11</t>
+  </si>
+  <si>
+    <t>a10</t>
+  </si>
+  <si>
+    <t>a9</t>
+  </si>
+  <si>
+    <t>a8</t>
+  </si>
+  <si>
+    <t>a7</t>
+  </si>
+  <si>
+    <t>a6</t>
+  </si>
+  <si>
+    <t>a5</t>
+  </si>
+  <si>
+    <t>a4</t>
+  </si>
+  <si>
+    <t>a3</t>
+  </si>
+  <si>
+    <t>a2</t>
+  </si>
+  <si>
+    <t>adc</t>
+  </si>
+  <si>
+    <t>Luz 7/M2</t>
+  </si>
+  <si>
+    <t>Luz 6/M1</t>
+  </si>
+  <si>
+    <t>Luz 2/Cuerpo 1</t>
+  </si>
+  <si>
+    <t>Luz 3/Cuerpo 3</t>
+  </si>
+  <si>
+    <t>Luz 5/Cuerpo 4</t>
+  </si>
+  <si>
+    <t>Luz 8/Error</t>
+  </si>
+  <si>
+    <t>Luz 16Cuerpo 2</t>
+  </si>
+  <si>
+    <t>Luz 11/Cuerpo 6</t>
+  </si>
+  <si>
+    <t>Luz 12/Cuerpo 5</t>
+  </si>
+  <si>
+    <t>D0.0/Unidad1</t>
+  </si>
+  <si>
+    <t>D0.2/Unidad3</t>
+  </si>
+  <si>
+    <t>D0.3/Unidad4</t>
+  </si>
+  <si>
+    <t>D0.1/unidad2</t>
+  </si>
+  <si>
+    <t>D2/Decena3</t>
+  </si>
+  <si>
+    <t>D1/Decena2</t>
+  </si>
+  <si>
+    <t>D3/Decena4</t>
+  </si>
+  <si>
+    <t>D0/Decena1</t>
+  </si>
+  <si>
+    <t>luz 17</t>
+  </si>
+  <si>
+    <t>luz18</t>
   </si>
 </sst>
 </file>
@@ -487,17 +568,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2990587F-D9E0-44A7-80F5-A2CDDA88A98C}">
-  <dimension ref="B2:D35"/>
+  <dimension ref="B2:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="12.21875" style="1" customWidth="1"/>
     <col min="3" max="3" width="13.77734375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" style="1"/>
+    <col min="4" max="4" width="14.109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
@@ -684,7 +765,7 @@
         <v>27</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
@@ -695,7 +776,7 @@
         <v>28</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
@@ -706,7 +787,7 @@
         <v>29</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
@@ -717,7 +798,7 @@
         <v>30</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
@@ -728,7 +809,7 @@
         <v>31</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
@@ -739,7 +820,7 @@
         <v>32</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
@@ -750,7 +831,7 @@
         <v>33</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>24</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.3">
@@ -761,7 +842,7 @@
         <v>34</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.3">
@@ -772,7 +853,7 @@
         <v>39</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.3">
@@ -783,7 +864,7 @@
         <v>40</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.3">
@@ -794,7 +875,7 @@
         <v>41</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.3">
@@ -805,7 +886,7 @@
         <v>42</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.3">
@@ -816,7 +897,7 @@
         <v>43</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.3">
@@ -827,7 +908,7 @@
         <v>44</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.3">
@@ -838,7 +919,7 @@
         <v>45</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.3">
@@ -849,7 +930,7 @@
         <v>46</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.3">
@@ -860,18 +941,169 @@
         <v>47</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B35" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C35" s="1">
         <v>48</v>
       </c>
       <c r="D35" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B36" s="1">
+        <v>4</v>
+      </c>
+      <c r="C36" s="1">
+        <v>49</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B37" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C37" s="1">
+        <v>1</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B38" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C38" s="1">
+        <v>2</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B39" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C39" s="1">
+        <v>3</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B40" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C40" s="1">
+        <v>4</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B41" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C41" s="1">
+        <v>5</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B42" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C42" s="1">
+        <v>6</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B43" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C43" s="1">
+        <v>7</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B44" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C44" s="1">
+        <v>8</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B45" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C45" s="1">
+        <v>9</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B46" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C46" s="1">
+        <v>10</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B47" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C47" s="1">
+        <v>11</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B48" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C48" s="1">
+        <v>12</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B49" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>